<commit_message>
Update Time log and Project Timeline.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Time log and Project Timeline.xlsx
+++ b/Documents/Time log and Project Timeline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4435487C-17C9-4537-99AA-3DA8653AEA2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3074914-5E5C-4E11-8051-E069F5267888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Task 3</t>
   </si>
@@ -60,15 +60,6 @@
   </si>
   <si>
     <t>This is an empty row</t>
-  </si>
-  <si>
-    <t>No. Days</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Assigned To</t>
   </si>
   <si>
     <t>Progress</t>
@@ -96,9 +87,6 @@
   </si>
   <si>
     <t>Legend:</t>
-  </si>
-  <si>
-    <t>Unassigned</t>
   </si>
   <si>
     <t>Milestone Description</t>
@@ -173,9 +161,6 @@
     <t>Presentation or exam Preperation</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
     <t>PROJECT 1</t>
   </si>
   <si>
@@ -198,6 +183,15 @@
   </si>
   <si>
     <t>created spreadsheet and separated some of the projects on git hub into sepatate to-do lists</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>End</t>
   </si>
 </sst>
 </file>
@@ -353,7 +347,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -385,31 +379,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -605,7 +593,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -734,10 +722,14 @@
     <xf numFmtId="165" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
@@ -753,21 +745,20 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="8" xfId="9" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="11" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -785,6 +776,15 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="29">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1068,15 +1068,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -1356,7 +1347,7 @@
                   <a14:compatExt spid="_x0000_s6149"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005180000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1397,12 +1388,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{EE48C34E-B98C-4BBA-90C8-388E8655DD6D}" name="Milestone Description" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{B8ACC97F-C189-49BA-91CF-CB5671185BCF}" name="Category" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{5419FA1B-A035-4F0A-9257-1AA4BCB5E6CF}" name="Assigned To" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{EE48C34E-B98C-4BBA-90C8-388E8655DD6D}" name="Milestone Description" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{B8ACC97F-C189-49BA-91CF-CB5671185BCF}" name=" " dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{5419FA1B-A035-4F0A-9257-1AA4BCB5E6CF}" name="  " dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{A60A6524-18F0-48B7-BB3C-2F4A35799FF7}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{59612C1F-9AAB-483B-A6A5-3563E9D77941}" name="Start" dataCellStyle="Date"/>
-    <tableColumn id="6" xr3:uid="{012C59F1-49D4-4A67-B8DD-855C6581FD6A}" name="No. Days" dataCellStyle="Comma [0]"/>
+    <tableColumn id="6" xr3:uid="{012C59F1-49D4-4A67-B8DD-855C6581FD6A}" name="End" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1686,51 +1677,51 @@
   <cols>
     <col min="1" max="1" width="16.08984375" customWidth="1"/>
     <col min="2" max="2" width="16.7265625" customWidth="1"/>
-    <col min="3" max="3" width="44.54296875" style="64" customWidth="1"/>
+    <col min="3" max="3" width="44.54296875" style="54" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="64" t="s">
-        <v>42</v>
+      <c r="C1" s="54" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="63">
+      <c r="A2" s="53">
         <v>0.29329861111111111</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="64" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="63">
+      <c r="A3" s="53">
         <v>0.37663194444444442</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="64" t="s">
-        <v>44</v>
+        <v>36</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="63">
+      <c r="A4" s="53">
         <v>0.37663194444444442</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="64" t="s">
-        <v>46</v>
+        <v>40</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1746,8 +1737,8 @@
   </sheetPr>
   <dimension ref="A1:BL18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="78" zoomScaleNormal="10" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B2" zoomScale="78" zoomScaleNormal="10" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1766,17 +1757,17 @@
   <sheetData>
     <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="1"/>
       <c r="F1"/>
       <c r="G1" s="7"/>
       <c r="I1" s="40" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J1" s="8"/>
       <c r="K1" s="20"/>
@@ -1805,70 +1796,68 @@
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="F2" s="23"/>
       <c r="G2" s="21"/>
-      <c r="I2" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="N2" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
+      <c r="I2" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="N2" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
       <c r="R2" s="20"/>
-      <c r="S2" s="61" t="s">
-        <v>14</v>
-      </c>
-      <c r="T2" s="61"/>
-      <c r="U2" s="61"/>
-      <c r="V2" s="61"/>
+      <c r="S2" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
       <c r="W2" s="20"/>
-      <c r="X2" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y2" s="52"/>
-      <c r="Z2" s="52"/>
-      <c r="AA2" s="52"/>
+      <c r="X2" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
       <c r="AB2" s="20"/>
-      <c r="AC2" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
-      <c r="AF2" s="53"/>
+      <c r="AC2" s="61"/>
+      <c r="AD2" s="61"/>
+      <c r="AE2" s="61"/>
+      <c r="AF2" s="61"/>
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
-      <c r="D3" s="54" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="57">
+      <c r="D3" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="57"/>
+      <c r="F3" s="59">
         <v>44232</v>
       </c>
-      <c r="G3" s="58"/>
+      <c r="G3" s="60"/>
       <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="55"/>
+        <v>20</v>
+      </c>
+      <c r="D4" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="57"/>
       <c r="F4" s="45">
         <v>0</v>
       </c>
@@ -1955,15 +1944,15 @@
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
+        <v>21</v>
+      </c>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
       <c r="I5" s="49">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
         <v>44232</v>
@@ -2191,7 +2180,7 @@
     </row>
     <row r="6" spans="1:64" s="20" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B6" s="35"/>
       <c r="C6" s="35"/>
@@ -2259,25 +2248,25 @@
     </row>
     <row r="7" spans="1:64" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C7" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>12</v>
-      </c>
       <c r="G7" s="29" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="25" t="str">
@@ -2507,7 +2496,7 @@
     </row>
     <row r="8" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B8" s="41"/>
       <c r="C8" s="30"/>
@@ -2575,35 +2564,35 @@
     <row r="9" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14"/>
       <c r="B9" s="42" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C9" s="34"/>
-      <c r="D9" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="62">
+      <c r="D9" s="34"/>
+      <c r="E9" s="31">
+        <v>0</v>
+      </c>
+      <c r="F9" s="52">
         <v>0.20996527777777776</v>
       </c>
       <c r="G9" s="33"/>
       <c r="H9" s="26"/>
-      <c r="I9" s="38" t="str">
+      <c r="I9" s="65" t="str">
         <f t="shared" ref="I9:X15" ca="1" si="6">IF(AND($C9="Goal",I$5&gt;=$F9,I$5&lt;=$F9+$G9-1),2,IF(AND($C9="Milestone",I$5&gt;=$F9,I$5&lt;=$F9+$G9-1),1,""))</f>
         <v/>
       </c>
-      <c r="J9" s="38" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="K9" s="38" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="L9" s="38" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v/>
-      </c>
-      <c r="M9" s="38" t="str">
+      <c r="J9" s="65" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="K9" s="65" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="L9" s="65" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v/>
+      </c>
+      <c r="M9" s="65" t="str">
         <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
@@ -2815,14 +2804,14 @@
     <row r="10" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14"/>
       <c r="B10" s="41" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
       <c r="E10" s="31">
         <v>0</v>
       </c>
-      <c r="F10" s="62">
+      <c r="F10" s="52">
         <v>0.37663194444444442</v>
       </c>
       <c r="G10" s="33"/>
@@ -2843,7 +2832,7 @@
         <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
-      <c r="M10" s="38" t="str">
+      <c r="M10" s="65" t="str">
         <f t="shared" ca="1" si="6"/>
         <v/>
       </c>
@@ -4001,7 +3990,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C15" s="34"/>
       <c r="D15" s="34"/>
@@ -4236,10 +4225,10 @@
     </row>
     <row r="16" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
@@ -4339,56 +4328,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:BL16">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:AM4">
-    <cfRule type="expression" dxfId="12" priority="7">
+    <cfRule type="expression" dxfId="15" priority="7">
       <formula>I$5&lt;=EOMONTH($I$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:BL4">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="14" priority="3">
       <formula>AND(J$5&lt;=EOMONTH($I$5,2),J$5&gt;EOMONTH($I$5,0),J$5&gt;EOMONTH($I$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:BL4">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND(I$5&lt;=EOMONTH($I$5,1),I$5&gt;EOMONTH($I$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:BL15">
-    <cfRule type="expression" dxfId="9" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="24" stopIfTrue="1">
       <formula>AND($C8="Low Risk",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="43" stopIfTrue="1">
       <formula>AND($C8="High Risk",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="61" stopIfTrue="1">
       <formula>AND($C8="On Track",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="62" stopIfTrue="1">
       <formula>AND($C8="Med Risk",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="63" stopIfTrue="1">
       <formula>AND(LEN($C8)=0,I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:BL16">
-    <cfRule type="expression" dxfId="4" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="71" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="72" stopIfTrue="1">
       <formula>AND(#REF!="High Risk",I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="73" stopIfTrue="1">
       <formula>AND(#REF!="On Track",I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="74" stopIfTrue="1">
       <formula>AND(#REF!="Med Risk",I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="75" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,I$5&gt;=#REF!,I$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4522,7 +4511,7 @@
     </row>
     <row r="2" spans="1:1" ht="84.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4532,12 +4521,12 @@
     </row>
     <row r="4" spans="1:1" s="10" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Time log variables added
Why what was done was done and what else needs doing in relation to what was done
</commit_message>
<xml_diff>
--- a/Documents/Time log and Project Timeline.xlsx
+++ b/Documents/Time log and Project Timeline.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5A5068-6B70-443D-BA32-56EE5FF98366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1DAB10-E912-45B3-B1F3-E6D6D205BB41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Task 3</t>
   </si>
@@ -208,14 +208,20 @@
   <si>
     <t>Added notes to jupyter notebook. Filtered vehicle and casualties tables according to Birmingham</t>
   </si>
+  <si>
+    <t>Does anything else need doing relating to this?</t>
+  </si>
+  <si>
+    <t>Why this was done?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="d"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="d"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -591,7 +597,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="1" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
@@ -719,22 +725,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
@@ -1682,10 +1688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2CC03F1-69F5-44F9-B6AB-0FB9DFF6FAEC}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1693,9 +1699,11 @@
     <col min="1" max="1" width="16.08984375" customWidth="1"/>
     <col min="2" max="2" width="16.7265625" customWidth="1"/>
     <col min="3" max="3" width="44.54296875" style="54" customWidth="1"/>
+    <col min="4" max="4" width="55.453125" customWidth="1"/>
+    <col min="5" max="5" width="48.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -1705,8 +1713,14 @@
       <c r="C1" s="54" t="s">
         <v>37</v>
       </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="53">
         <v>0.29329861111111111</v>
       </c>
@@ -1717,7 +1731,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="53">
         <v>0.37663194444444442</v>
       </c>
@@ -1728,7 +1742,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="53">
         <v>0.37663194444444442</v>
       </c>
@@ -1739,7 +1753,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="53">
         <v>0.45996527777777779</v>
       </c>
@@ -1750,7 +1764,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="53">
         <v>0.45996527777777779</v>
       </c>
@@ -1761,7 +1775,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="53">
         <v>0.50163194444444448</v>
       </c>

</xml_diff>